<commit_message>
Modificaciones enunciado lab 5 2023-20
</commit_message>
<xml_diff>
--- a/Docs/ISIS1225 - TablasDatos-Lab4-5.xlsx
+++ b/Docs/ISIS1225 - TablasDatos-Lab4-5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4428830306c10d/Documents/GitHub/ISIS1225DEVS/ISIS1225-SampleSorts/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd4428830306c10d/Documents/GitHub/ISIS1225DEVS/ISIS1225-SampleRecursion/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="165" documentId="8_{D9F3EF8E-9153-42A5-8ACF-6285D7DFF156}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{98C2BCE3-F10F-468E-A683-4219F3755E9A}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="19440" windowHeight="11640" activeTab="1" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15586" firstSheet="2" activeTab="7" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab4-5" sheetId="1" r:id="rId1"/>
@@ -128,27 +128,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -10630,7 +10624,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{BF2A59F4-6CD8-490D-818C-7B3BB3F2B140}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10641,7 +10635,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EAD1D623-F0B6-4C1A-913F-35E2F001B69E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="33" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10685,7 +10679,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{C0D6BB1E-4928-4857-A0CD-C818D0A5A6F2}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10696,7 +10690,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B3AE6AD4-6EB7-44ED-A987-5D4A68E7E10B}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -10707,7 +10701,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="19482955" cy="14143182"/>
+    <xdr:ext cx="8666238" cy="6289524"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10740,7 +10734,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="19482955" cy="14143182"/>
+    <xdr:ext cx="8657729" cy="6282566"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10872,7 +10866,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8659519" cy="6284148"/>
+    <xdr:ext cx="8657729" cy="6282566"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -10905,7 +10899,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8657729" cy="6282566"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11303,34 +11297,34 @@
     <col min="6" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="8" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" s="6" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A2" s="4">
+      <c r="A2" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
@@ -11356,10 +11350,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>0.05</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
@@ -11375,20 +11369,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>2023.2207481840321</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>445</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>481.8892790030352</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>0.1</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
@@ -11404,20 +11398,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>9920</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>1720</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>484.2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0.2</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
@@ -11433,20 +11427,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>47965.915742002711</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>6820</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>489.24288398785916</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>0.3</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
@@ -11462,20 +11456,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>119714.68497823011</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>15320</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>494.60390926982257</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>0.5</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
@@ -11491,20 +11485,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>376285.42505688418</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>42520</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>505.8927900303521</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>0.8</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
@@ -11520,20 +11514,20 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>1072501.4458375969</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>108820</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>523.71460785430975</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <f>Table1[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
@@ -11549,43 +11543,43 @@
         <f>(1.1*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]))^2)/1000+20</f>
         <v>1760020.0000000002</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f>(1.7*Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]^2)/1000+20</f>
         <v>170020</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <f>(1.4*(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]]*LOG10(Table1[[#This Row],[Tamaño de la muestra (ARRAY_LIST)]])))/1000+120*4</f>
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="8" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:7" s="6" customFormat="1" ht="27.35" x14ac:dyDescent="0.4">
+      <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>50</v>
       </c>
@@ -11611,10 +11605,10 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>0.05</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>500</v>
       </c>
@@ -11640,175 +11634,175 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>0.1</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>1000</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>1350</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>1650</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>10850</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>1850</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>604.5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>0.2</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>2000</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>5250</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>6450</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>52354.635354912039</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>7250</v>
       </c>
-      <c r="G16" s="5">
+      <c r="G16" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>609.90308998699197</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A17" s="4">
+      <c r="A17" s="3">
         <v>0.3</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>3000</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>11750</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>14450</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>130626.01997625102</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>16250</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>615.64704564623844</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>0.5</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>5000</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>32550</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>40050</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>410521.37278932816</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>45050</v>
       </c>
-      <c r="G18" s="5">
+      <c r="G18" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>627.74227503252018</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>0.8</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>8000</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>83250</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>102450</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>1170029.7590955601</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>115250</v>
       </c>
-      <c r="G19" s="5">
+      <c r="G19" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>646.83707984390333</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.5">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>1</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <f>Table13[[#This Row],[Porcentaje de la muestra '[pct']]]*10000</f>
         <v>10000</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <f>(1.3*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>130050</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <f>(1.6*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>160050</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <f>(1.2*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]))^2)/1000+50</f>
         <v>1920050</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <f>(1.8*Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]^2)/1000+50</f>
         <v>180050</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <f>(1.5*(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]]*LOG10(Table13[[#This Row],[Tamaño de la muestra (LINKED_LIST)]])))/1000+150*4</f>
         <v>660</v>
       </c>
@@ -11823,15 +11817,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <SharedWithUsers xmlns="85e30bcc-d76c-4413-8e4d-2dce22fb0743">
@@ -11938,6 +11923,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12158,14 +12152,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -12178,6 +12164,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>